<commit_message>
op dit moment kan mijn code alle data inladen, en vervolgens alle afstanden tussen alle vliegvelden i en j berekenen, en ook de afstanden alleen van en naar frankfurt de hub
</commit_message>
<xml_diff>
--- a/data/DemandGroup16.xlsx
+++ b/data/DemandGroup16.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gijsvdklink/Documents/Airline planning and optimisation /Assignment_1/airline planning 2/Airline_planning/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8614C9-52DA-8F4B-97AF-67F0C500124F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A414416C-9727-984D-83EF-38DB7F18EF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="2" xr2:uid="{FB73AE3F-7B15-3D43-954F-214C39B187E1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20100" activeTab="2" xr2:uid="{FB73AE3F-7B15-3D43-954F-214C39B187E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Group 16" sheetId="1" r:id="rId1"/>
@@ -2383,10 +2383,13 @@
   <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -2788,7 +2791,7 @@
   <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>